<commit_message>
update data dictionary add readGenotypes
</commit_message>
<xml_diff>
--- a/collection_data_dictionary_v2.xlsx
+++ b/collection_data_dictionary_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/repos/easyfulcrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8BE8CC1-EF2A-E24C-91EC-3EEA0E79E3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECE0630-31BE-C044-978B-9593F93678EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20120" xr2:uid="{89EDBE6F-D649-2C47-B9B8-5FFDEB3898C0}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20140" xr2:uid="{89EDBE6F-D649-2C47-B9B8-5FFDEB3898C0}"/>
   </bookViews>
   <sheets>
     <sheet name="fulcrum_dat.Rda_dic" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="188">
   <si>
     <t>isolation_by</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>genotying data</t>
+  </si>
+  <si>
+    <t>trail where collected</t>
   </si>
 </sst>
 </file>
@@ -741,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -791,6 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,7 +1112,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,6 +1326,9 @@
       <c r="A16" s="12"/>
       <c r="B16" s="25" t="s">
         <v>160</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>